<commit_message>
Added cell style tests
</commit_message>
<xml_diff>
--- a/EZSpreadsheet.Tests/ExpectedFiles/ShouldAddCellsInSameColumn.xlsx
+++ b/EZSpreadsheet.Tests/ExpectedFiles/ShouldAddCellsInSameColumn.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" r:id="R4484ef3a84204271"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" r:id="R35007c499c1f4d34"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -30,10 +30,18 @@
   </x:fills>
   <x:borders count="1">
     <x:border>
-      <x:left style="none"/>
-      <x:right style="none"/>
-      <x:top style="none"/>
-      <x:bottom style="none"/>
+      <x:left style="none">
+        <x:color indexed="0"/>
+      </x:left>
+      <x:right style="none">
+        <x:color indexed="0"/>
+      </x:right>
+      <x:top style="none">
+        <x:color indexed="0"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color indexed="0"/>
+      </x:bottom>
     </x:border>
   </x:borders>
   <x:cellXfs count="1">

</xml_diff>